<commit_message>
pcb start and hotswap boyz
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spide\Documents\KiCAD\Installation-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB04B93-3ED9-4B57-9FC1-812E898201D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E6CACA-5D7B-4EE9-BB5B-6581229FF627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1613" uniqueCount="594">
   <si>
     <t>Refs</t>
   </si>
@@ -1129,9 +1129,6 @@
     <t>MX1</t>
   </si>
   <si>
-    <t>MX_Only:MXOnly-1U-Hotswap-Antishear</t>
-  </si>
-  <si>
     <t>ESC</t>
   </si>
   <si>
@@ -1799,6 +1796,12 @@
   </si>
   <si>
     <t>Crystal_SMD_3225-4pin_3.2x2.5mm</t>
+  </si>
+  <si>
+    <t>Kailh_socket_MX</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -2138,11 +2141,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D448"/>
+  <dimension ref="A1:P448"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P11" sqref="P11"/>
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2169,7 +2172,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -2183,7 +2186,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -2197,7 +2200,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -2211,7 +2214,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -2225,7 +2228,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -2239,7 +2242,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -2253,7 +2256,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -2267,7 +2270,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -2281,7 +2284,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -2295,7 +2298,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -2309,7 +2312,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -2323,7 +2326,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -2337,7 +2340,7 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -2351,7 +2354,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -2365,7 +2368,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -2379,7 +2382,7 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -2393,7 +2396,7 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
@@ -2407,7 +2410,7 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
@@ -2421,7 +2424,7 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
@@ -2435,7 +2438,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
@@ -2449,7 +2452,7 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
@@ -2463,7 +2466,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
@@ -2477,7 +2480,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
@@ -2491,7 +2494,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
@@ -2505,7 +2508,7 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
@@ -2519,7 +2522,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
@@ -2533,7 +2536,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
@@ -2547,7 +2550,7 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -2561,7 +2564,7 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
@@ -2575,7 +2578,7 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
@@ -2589,7 +2592,7 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -2603,7 +2606,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
@@ -2617,7 +2620,7 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D34" t="s">
         <v>9</v>
@@ -2631,7 +2634,7 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D35" t="s">
         <v>9</v>
@@ -2645,7 +2648,7 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D36" t="s">
         <v>20</v>
@@ -2659,7 +2662,7 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D37" t="s">
         <v>9</v>
@@ -2673,7 +2676,7 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D38" t="s">
         <v>9</v>
@@ -2687,7 +2690,7 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
@@ -2701,7 +2704,7 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
@@ -2715,7 +2718,7 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
@@ -2729,7 +2732,7 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
@@ -2743,7 +2746,7 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
@@ -2757,7 +2760,7 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
@@ -2771,7 +2774,7 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D45" t="s">
         <v>9</v>
@@ -2785,7 +2788,7 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>
@@ -2799,7 +2802,7 @@
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D47" t="s">
         <v>20</v>
@@ -2813,7 +2816,7 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
@@ -2827,7 +2830,7 @@
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D49" t="s">
         <v>9</v>
@@ -2841,7 +2844,7 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D50" t="s">
         <v>9</v>
@@ -2855,7 +2858,7 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D51" t="s">
         <v>6</v>
@@ -2869,7 +2872,7 @@
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D52" t="s">
         <v>6</v>
@@ -2883,7 +2886,7 @@
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D53" t="s">
         <v>60</v>
@@ -2897,7 +2900,7 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D54" t="s">
         <v>20</v>
@@ -2911,7 +2914,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
@@ -2925,7 +2928,7 @@
         <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D56" t="s">
         <v>64</v>
@@ -2939,7 +2942,7 @@
         <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D57" t="s">
         <v>64</v>
@@ -2953,7 +2956,7 @@
         <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D58" t="s">
         <v>6</v>
@@ -2967,7 +2970,7 @@
         <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D59" t="s">
         <v>6</v>
@@ -2981,7 +2984,7 @@
         <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D60" t="s">
         <v>20</v>
@@ -2995,7 +2998,7 @@
         <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D61" t="s">
         <v>9</v>
@@ -3009,7 +3012,7 @@
         <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D62" t="s">
         <v>9</v>
@@ -3023,7 +3026,7 @@
         <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
@@ -3037,7 +3040,7 @@
         <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D64" t="s">
         <v>9</v>
@@ -3051,7 +3054,7 @@
         <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D65" t="s">
         <v>9</v>
@@ -3065,7 +3068,7 @@
         <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D66" t="s">
         <v>9</v>
@@ -3079,7 +3082,7 @@
         <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D67" t="s">
         <v>9</v>
@@ -3093,7 +3096,7 @@
         <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D68" t="s">
         <v>9</v>
@@ -3107,7 +3110,7 @@
         <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D69" t="s">
         <v>9</v>
@@ -3121,7 +3124,7 @@
         <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D70" t="s">
         <v>6</v>
@@ -3135,7 +3138,7 @@
         <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D71" t="s">
         <v>80</v>
@@ -3149,7 +3152,7 @@
         <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D72" t="s">
         <v>9</v>
@@ -3163,7 +3166,7 @@
         <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D73" t="s">
         <v>9</v>
@@ -3177,7 +3180,7 @@
         <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D74" t="s">
         <v>80</v>
@@ -3191,7 +3194,7 @@
         <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D75" t="s">
         <v>9</v>
@@ -3205,7 +3208,7 @@
         <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D76" t="s">
         <v>9</v>
@@ -3219,7 +3222,7 @@
         <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D77" t="s">
         <v>9</v>
@@ -3233,7 +3236,7 @@
         <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D78" t="s">
         <v>9</v>
@@ -3247,7 +3250,7 @@
         <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D79" t="s">
         <v>9</v>
@@ -3261,7 +3264,7 @@
         <v>5</v>
       </c>
       <c r="C80" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D80" t="s">
         <v>9</v>
@@ -3275,7 +3278,7 @@
         <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D81" t="s">
         <v>91</v>
@@ -3289,7 +3292,7 @@
         <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D82" t="s">
         <v>9</v>
@@ -3303,7 +3306,7 @@
         <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D83" t="s">
         <v>9</v>
@@ -3317,7 +3320,7 @@
         <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D84" t="s">
         <v>6</v>
@@ -3331,7 +3334,7 @@
         <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D85" t="s">
         <v>96</v>
@@ -3345,7 +3348,7 @@
         <v>5</v>
       </c>
       <c r="C86" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D86" t="s">
         <v>96</v>
@@ -3359,7 +3362,7 @@
         <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D87" t="s">
         <v>96</v>
@@ -3373,7 +3376,7 @@
         <v>5</v>
       </c>
       <c r="C88" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D88" t="s">
         <v>96</v>
@@ -3387,7 +3390,7 @@
         <v>5</v>
       </c>
       <c r="C89" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D89" t="s">
         <v>9</v>
@@ -3401,7 +3404,7 @@
         <v>5</v>
       </c>
       <c r="C90" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D90" t="s">
         <v>9</v>
@@ -3415,7 +3418,7 @@
         <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D91" t="s">
         <v>9</v>
@@ -3429,7 +3432,7 @@
         <v>5</v>
       </c>
       <c r="C92" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D92" t="s">
         <v>6</v>
@@ -3443,7 +3446,7 @@
         <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D93" t="s">
         <v>9</v>
@@ -3457,7 +3460,7 @@
         <v>5</v>
       </c>
       <c r="C94" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D94" t="s">
         <v>9</v>
@@ -3471,7 +3474,7 @@
         <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D95" t="s">
         <v>9</v>
@@ -3485,7 +3488,7 @@
         <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D96" t="s">
         <v>9</v>
@@ -3499,7 +3502,7 @@
         <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D97" t="s">
         <v>9</v>
@@ -3513,7 +3516,7 @@
         <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D98" t="s">
         <v>9</v>
@@ -3527,7 +3530,7 @@
         <v>5</v>
       </c>
       <c r="C99" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D99" t="s">
         <v>9</v>
@@ -3541,7 +3544,7 @@
         <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D100" t="s">
         <v>9</v>
@@ -3555,7 +3558,7 @@
         <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D101" t="s">
         <v>9</v>
@@ -3569,7 +3572,7 @@
         <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D102" t="s">
         <v>9</v>
@@ -3583,7 +3586,7 @@
         <v>5</v>
       </c>
       <c r="C103" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D103" t="s">
         <v>91</v>
@@ -3597,7 +3600,7 @@
         <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D104" t="s">
         <v>9</v>
@@ -3611,7 +3614,7 @@
         <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D105" t="s">
         <v>9</v>
@@ -3625,7 +3628,7 @@
         <v>5</v>
       </c>
       <c r="C106" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D106" t="s">
         <v>9</v>
@@ -3639,7 +3642,7 @@
         <v>5</v>
       </c>
       <c r="C107" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D107" t="s">
         <v>9</v>
@@ -3653,7 +3656,7 @@
         <v>5</v>
       </c>
       <c r="C108" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D108" t="s">
         <v>9</v>
@@ -3667,7 +3670,7 @@
         <v>5</v>
       </c>
       <c r="C109" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D109" t="s">
         <v>9</v>
@@ -3681,7 +3684,7 @@
         <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D110" t="s">
         <v>9</v>
@@ -3695,7 +3698,7 @@
         <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D111" t="s">
         <v>9</v>
@@ -3709,7 +3712,7 @@
         <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D112" t="s">
         <v>9</v>
@@ -3723,7 +3726,7 @@
         <v>5</v>
       </c>
       <c r="C113" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D113" t="s">
         <v>9</v>
@@ -3737,7 +3740,7 @@
         <v>5</v>
       </c>
       <c r="C114" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D114" t="s">
         <v>126</v>
@@ -3751,7 +3754,7 @@
         <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D115" t="s">
         <v>9</v>
@@ -3765,7 +3768,7 @@
         <v>5</v>
       </c>
       <c r="C116" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D116" t="s">
         <v>9</v>
@@ -3779,7 +3782,7 @@
         <v>5</v>
       </c>
       <c r="C117" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D117" t="s">
         <v>9</v>
@@ -3793,7 +3796,7 @@
         <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D118" t="s">
         <v>9</v>
@@ -3807,7 +3810,7 @@
         <v>5</v>
       </c>
       <c r="C119" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D119" t="s">
         <v>9</v>
@@ -3821,7 +3824,7 @@
         <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D120" t="s">
         <v>9</v>
@@ -3835,7 +3838,7 @@
         <v>5</v>
       </c>
       <c r="C121" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D121" t="s">
         <v>9</v>
@@ -3849,7 +3852,7 @@
         <v>5</v>
       </c>
       <c r="C122" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D122" t="s">
         <v>9</v>
@@ -3863,7 +3866,7 @@
         <v>5</v>
       </c>
       <c r="C123" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D123" t="s">
         <v>9</v>
@@ -3877,7 +3880,7 @@
         <v>5</v>
       </c>
       <c r="C124" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D124" t="s">
         <v>9</v>
@@ -3891,7 +3894,7 @@
         <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D125" t="s">
         <v>138</v>
@@ -3905,7 +3908,7 @@
         <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D126" t="s">
         <v>9</v>
@@ -3919,7 +3922,7 @@
         <v>5</v>
       </c>
       <c r="C127" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D127" t="s">
         <v>9</v>
@@ -3933,7 +3936,7 @@
         <v>5</v>
       </c>
       <c r="C128" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D128" t="s">
         <v>9</v>
@@ -3947,7 +3950,7 @@
         <v>5</v>
       </c>
       <c r="C129" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D129" t="s">
         <v>9</v>
@@ -3961,7 +3964,7 @@
         <v>5</v>
       </c>
       <c r="C130" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D130" t="s">
         <v>9</v>
@@ -3975,7 +3978,7 @@
         <v>5</v>
       </c>
       <c r="C131" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D131" t="s">
         <v>9</v>
@@ -3989,7 +3992,7 @@
         <v>5</v>
       </c>
       <c r="C132" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D132" t="s">
         <v>9</v>
@@ -4003,7 +4006,7 @@
         <v>5</v>
       </c>
       <c r="C133" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D133" t="s">
         <v>9</v>
@@ -4017,7 +4020,7 @@
         <v>5</v>
       </c>
       <c r="C134" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D134" t="s">
         <v>9</v>
@@ -4031,7 +4034,7 @@
         <v>5</v>
       </c>
       <c r="C135" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D135" t="s">
         <v>9</v>
@@ -4045,7 +4048,7 @@
         <v>5</v>
       </c>
       <c r="C136" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D136" t="s">
         <v>6</v>
@@ -4059,7 +4062,7 @@
         <v>5</v>
       </c>
       <c r="C137" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D137" t="s">
         <v>9</v>
@@ -4073,7 +4076,7 @@
         <v>5</v>
       </c>
       <c r="C138" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D138" t="s">
         <v>9</v>
@@ -4087,7 +4090,7 @@
         <v>5</v>
       </c>
       <c r="C139" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D139" t="s">
         <v>9</v>
@@ -4101,7 +4104,7 @@
         <v>5</v>
       </c>
       <c r="C140" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D140" t="s">
         <v>9</v>
@@ -4115,7 +4118,7 @@
         <v>5</v>
       </c>
       <c r="C141" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D141" t="s">
         <v>9</v>
@@ -4129,7 +4132,7 @@
         <v>5</v>
       </c>
       <c r="C142" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D142" t="s">
         <v>9</v>
@@ -4143,7 +4146,7 @@
         <v>5</v>
       </c>
       <c r="C143" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D143" t="s">
         <v>9</v>
@@ -4157,7 +4160,7 @@
         <v>5</v>
       </c>
       <c r="C144" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D144" t="s">
         <v>9</v>
@@ -4171,7 +4174,7 @@
         <v>5</v>
       </c>
       <c r="C145" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D145" t="s">
         <v>9</v>
@@ -4185,7 +4188,7 @@
         <v>5</v>
       </c>
       <c r="C146" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D146" t="s">
         <v>9</v>
@@ -4213,7 +4216,7 @@
         <v>5</v>
       </c>
       <c r="C148" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D148" t="s">
         <v>165</v>
@@ -4227,7 +4230,7 @@
         <v>5</v>
       </c>
       <c r="C149" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D149" t="s">
         <v>165</v>
@@ -4241,7 +4244,7 @@
         <v>5</v>
       </c>
       <c r="C150" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D150" t="s">
         <v>165</v>
@@ -4255,7 +4258,7 @@
         <v>5</v>
       </c>
       <c r="C151" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D151" t="s">
         <v>165</v>
@@ -4269,7 +4272,7 @@
         <v>5</v>
       </c>
       <c r="C152" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D152" t="s">
         <v>165</v>
@@ -4283,7 +4286,7 @@
         <v>5</v>
       </c>
       <c r="C153" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D153" t="s">
         <v>165</v>
@@ -4297,7 +4300,7 @@
         <v>5</v>
       </c>
       <c r="C154" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D154" t="s">
         <v>165</v>
@@ -4311,7 +4314,7 @@
         <v>5</v>
       </c>
       <c r="C155" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D155" t="s">
         <v>165</v>
@@ -4325,7 +4328,7 @@
         <v>5</v>
       </c>
       <c r="C156" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D156" t="s">
         <v>165</v>
@@ -4339,7 +4342,7 @@
         <v>5</v>
       </c>
       <c r="C157" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D157" t="s">
         <v>165</v>
@@ -4367,7 +4370,7 @@
         <v>5</v>
       </c>
       <c r="C159" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D159" t="s">
         <v>165</v>
@@ -4381,7 +4384,7 @@
         <v>5</v>
       </c>
       <c r="C160" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D160" t="s">
         <v>165</v>
@@ -4395,7 +4398,7 @@
         <v>5</v>
       </c>
       <c r="C161" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D161" t="s">
         <v>165</v>
@@ -4409,7 +4412,7 @@
         <v>5</v>
       </c>
       <c r="C162" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D162" t="s">
         <v>165</v>
@@ -4423,7 +4426,7 @@
         <v>5</v>
       </c>
       <c r="C163" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -4437,7 +4440,7 @@
         <v>5</v>
       </c>
       <c r="C164" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D164" t="s">
         <v>165</v>
@@ -4451,7 +4454,7 @@
         <v>5</v>
       </c>
       <c r="C165" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D165" t="s">
         <v>165</v>
@@ -4465,7 +4468,7 @@
         <v>5</v>
       </c>
       <c r="C166" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D166" t="s">
         <v>165</v>
@@ -4479,7 +4482,7 @@
         <v>5</v>
       </c>
       <c r="C167" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D167" t="s">
         <v>165</v>
@@ -4493,7 +4496,7 @@
         <v>5</v>
       </c>
       <c r="C168" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D168" t="s">
         <v>165</v>
@@ -4521,7 +4524,7 @@
         <v>5</v>
       </c>
       <c r="C170" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D170" t="s">
         <v>165</v>
@@ -4535,7 +4538,7 @@
         <v>5</v>
       </c>
       <c r="C171" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D171" t="s">
         <v>165</v>
@@ -4549,7 +4552,7 @@
         <v>5</v>
       </c>
       <c r="C172" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D172" t="s">
         <v>165</v>
@@ -4563,7 +4566,7 @@
         <v>5</v>
       </c>
       <c r="C173" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D173" t="s">
         <v>165</v>
@@ -4577,7 +4580,7 @@
         <v>5</v>
       </c>
       <c r="C174" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D174" t="s">
         <v>165</v>
@@ -4591,7 +4594,7 @@
         <v>5</v>
       </c>
       <c r="C175" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D175" t="s">
         <v>165</v>
@@ -4605,7 +4608,7 @@
         <v>5</v>
       </c>
       <c r="C176" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D176" t="s">
         <v>165</v>
@@ -4619,7 +4622,7 @@
         <v>5</v>
       </c>
       <c r="C177" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D177" t="s">
         <v>165</v>
@@ -4633,7 +4636,7 @@
         <v>5</v>
       </c>
       <c r="C178" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D178" t="s">
         <v>165</v>
@@ -4647,7 +4650,7 @@
         <v>5</v>
       </c>
       <c r="C179" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D179" t="s">
         <v>165</v>
@@ -4675,7 +4678,7 @@
         <v>5</v>
       </c>
       <c r="C181" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D181" t="s">
         <v>165</v>
@@ -4689,7 +4692,7 @@
         <v>5</v>
       </c>
       <c r="C182" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D182" t="s">
         <v>165</v>
@@ -4703,7 +4706,7 @@
         <v>5</v>
       </c>
       <c r="C183" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D183" t="s">
         <v>165</v>
@@ -4717,7 +4720,7 @@
         <v>5</v>
       </c>
       <c r="C184" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D184" t="s">
         <v>165</v>
@@ -4731,7 +4734,7 @@
         <v>5</v>
       </c>
       <c r="C185" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D185" t="s">
         <v>165</v>
@@ -4745,7 +4748,7 @@
         <v>5</v>
       </c>
       <c r="C186" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D186" t="s">
         <v>165</v>
@@ -4759,7 +4762,7 @@
         <v>5</v>
       </c>
       <c r="C187" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D187" t="s">
         <v>165</v>
@@ -4773,7 +4776,7 @@
         <v>5</v>
       </c>
       <c r="C188" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D188" t="s">
         <v>165</v>
@@ -4787,7 +4790,7 @@
         <v>5</v>
       </c>
       <c r="C189" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D189" t="s">
         <v>165</v>
@@ -4801,7 +4804,7 @@
         <v>5</v>
       </c>
       <c r="C190" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D190" t="s">
         <v>165</v>
@@ -4829,7 +4832,7 @@
         <v>5</v>
       </c>
       <c r="C192" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D192" t="s">
         <v>165</v>
@@ -4843,7 +4846,7 @@
         <v>5</v>
       </c>
       <c r="C193" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D193" t="s">
         <v>165</v>
@@ -4857,7 +4860,7 @@
         <v>5</v>
       </c>
       <c r="C194" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D194" t="s">
         <v>165</v>
@@ -4871,7 +4874,7 @@
         <v>5</v>
       </c>
       <c r="C195" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D195" t="s">
         <v>165</v>
@@ -4885,7 +4888,7 @@
         <v>5</v>
       </c>
       <c r="C196" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D196" t="s">
         <v>165</v>
@@ -4899,7 +4902,7 @@
         <v>5</v>
       </c>
       <c r="C197" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D197" t="s">
         <v>165</v>
@@ -4913,7 +4916,7 @@
         <v>5</v>
       </c>
       <c r="C198" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D198" t="s">
         <v>165</v>
@@ -4927,7 +4930,7 @@
         <v>5</v>
       </c>
       <c r="C199" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D199" t="s">
         <v>165</v>
@@ -4941,7 +4944,7 @@
         <v>5</v>
       </c>
       <c r="C200" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D200" t="s">
         <v>165</v>
@@ -4955,7 +4958,7 @@
         <v>5</v>
       </c>
       <c r="C201" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D201" t="s">
         <v>165</v>
@@ -4983,7 +4986,7 @@
         <v>5</v>
       </c>
       <c r="C203" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D203" t="s">
         <v>165</v>
@@ -4997,7 +5000,7 @@
         <v>5</v>
       </c>
       <c r="C204" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D204" t="s">
         <v>165</v>
@@ -5011,7 +5014,7 @@
         <v>5</v>
       </c>
       <c r="C205" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D205" t="s">
         <v>165</v>
@@ -5025,7 +5028,7 @@
         <v>5</v>
       </c>
       <c r="C206" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D206" t="s">
         <v>165</v>
@@ -5039,7 +5042,7 @@
         <v>5</v>
       </c>
       <c r="C207" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D207" t="s">
         <v>165</v>
@@ -5053,7 +5056,7 @@
         <v>5</v>
       </c>
       <c r="C208" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D208" t="s">
         <v>165</v>
@@ -5067,7 +5070,7 @@
         <v>5</v>
       </c>
       <c r="C209" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D209" t="s">
         <v>165</v>
@@ -5081,7 +5084,7 @@
         <v>5</v>
       </c>
       <c r="C210" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D210" t="s">
         <v>165</v>
@@ -5095,7 +5098,7 @@
         <v>5</v>
       </c>
       <c r="C211" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D211" t="s">
         <v>165</v>
@@ -5109,7 +5112,7 @@
         <v>5</v>
       </c>
       <c r="C212" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D212" t="s">
         <v>165</v>
@@ -5123,7 +5126,7 @@
         <v>5</v>
       </c>
       <c r="C213" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D213" t="s">
         <v>165</v>
@@ -5137,7 +5140,7 @@
         <v>5</v>
       </c>
       <c r="C214" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D214" t="s">
         <v>165</v>
@@ -5151,7 +5154,7 @@
         <v>5</v>
       </c>
       <c r="C215" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D215" t="s">
         <v>165</v>
@@ -5165,7 +5168,7 @@
         <v>5</v>
       </c>
       <c r="C216" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D216" t="s">
         <v>165</v>
@@ -5179,7 +5182,7 @@
         <v>5</v>
       </c>
       <c r="C217" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D217" t="s">
         <v>165</v>
@@ -5193,7 +5196,7 @@
         <v>5</v>
       </c>
       <c r="C218" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D218" t="s">
         <v>165</v>
@@ -5207,7 +5210,7 @@
         <v>5</v>
       </c>
       <c r="C219" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D219" t="s">
         <v>165</v>
@@ -5221,7 +5224,7 @@
         <v>5</v>
       </c>
       <c r="C220" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D220" t="s">
         <v>165</v>
@@ -5235,7 +5238,7 @@
         <v>5</v>
       </c>
       <c r="C221" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D221" t="s">
         <v>165</v>
@@ -5249,7 +5252,7 @@
         <v>5</v>
       </c>
       <c r="C222" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D222" t="s">
         <v>165</v>
@@ -5263,7 +5266,7 @@
         <v>5</v>
       </c>
       <c r="C223" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D223" t="s">
         <v>165</v>
@@ -5277,7 +5280,7 @@
         <v>5</v>
       </c>
       <c r="C224" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D224" t="s">
         <v>165</v>
@@ -5291,7 +5294,7 @@
         <v>5</v>
       </c>
       <c r="C225" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D225" t="s">
         <v>165</v>
@@ -5305,7 +5308,7 @@
         <v>5</v>
       </c>
       <c r="C226" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D226" t="s">
         <v>165</v>
@@ -5319,7 +5322,7 @@
         <v>5</v>
       </c>
       <c r="C227" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D227" t="s">
         <v>165</v>
@@ -5333,7 +5336,7 @@
         <v>5</v>
       </c>
       <c r="C228" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D228" t="s">
         <v>165</v>
@@ -5347,7 +5350,7 @@
         <v>5</v>
       </c>
       <c r="C229" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D229" t="s">
         <v>165</v>
@@ -5361,7 +5364,7 @@
         <v>5</v>
       </c>
       <c r="C230" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D230" t="s">
         <v>165</v>
@@ -5375,7 +5378,7 @@
         <v>5</v>
       </c>
       <c r="C231" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D231" t="s">
         <v>165</v>
@@ -5389,7 +5392,7 @@
         <v>5</v>
       </c>
       <c r="C232" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D232" t="s">
         <v>165</v>
@@ -5403,7 +5406,7 @@
         <v>5</v>
       </c>
       <c r="C233" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D233" t="s">
         <v>165</v>
@@ -5417,7 +5420,7 @@
         <v>5</v>
       </c>
       <c r="C234" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D234" t="s">
         <v>165</v>
@@ -5439,7 +5442,7 @@
         <v>5</v>
       </c>
       <c r="C236" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D236" t="s">
         <v>258</v>
@@ -5453,7 +5456,7 @@
         <v>5</v>
       </c>
       <c r="C237" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D237" t="s">
         <v>258</v>
@@ -6554,51 +6557,51 @@
         <v>368</v>
       </c>
       <c r="C336" t="s">
+        <v>592</v>
+      </c>
+      <c r="D336" t="s">
         <v>369</v>
-      </c>
-      <c r="D336" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
+        <v>370</v>
+      </c>
+      <c r="C337" t="s">
+        <v>592</v>
+      </c>
+      <c r="D337" t="s">
         <v>371</v>
-      </c>
-      <c r="C337" t="s">
-        <v>369</v>
-      </c>
-      <c r="D337" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
+        <v>372</v>
+      </c>
+      <c r="C338" t="s">
+        <v>592</v>
+      </c>
+      <c r="D338" t="s">
         <v>373</v>
-      </c>
-      <c r="C338" t="s">
-        <v>369</v>
-      </c>
-      <c r="D338" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
+        <v>374</v>
+      </c>
+      <c r="C339" t="s">
+        <v>584</v>
+      </c>
+      <c r="D339" t="s">
         <v>375</v>
-      </c>
-      <c r="C339" t="s">
-        <v>585</v>
-      </c>
-      <c r="D339" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C340" t="s">
-        <v>369</v>
+        <v>592</v>
       </c>
       <c r="D340" t="s">
         <v>259</v>
@@ -6606,109 +6609,109 @@
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
+        <v>377</v>
+      </c>
+      <c r="C341" t="s">
+        <v>592</v>
+      </c>
+      <c r="D341" t="s">
         <v>378</v>
-      </c>
-      <c r="C341" t="s">
-        <v>369</v>
-      </c>
-      <c r="D341" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
+        <v>379</v>
+      </c>
+      <c r="C342" t="s">
+        <v>592</v>
+      </c>
+      <c r="D342" t="s">
         <v>380</v>
-      </c>
-      <c r="C342" t="s">
-        <v>369</v>
-      </c>
-      <c r="D342" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
+        <v>381</v>
+      </c>
+      <c r="C343" t="s">
+        <v>592</v>
+      </c>
+      <c r="D343" t="s">
         <v>382</v>
-      </c>
-      <c r="C343" t="s">
-        <v>369</v>
-      </c>
-      <c r="D343" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
+        <v>383</v>
+      </c>
+      <c r="C344" t="s">
+        <v>592</v>
+      </c>
+      <c r="D344" t="s">
         <v>384</v>
-      </c>
-      <c r="C344" t="s">
-        <v>369</v>
-      </c>
-      <c r="D344" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
+        <v>385</v>
+      </c>
+      <c r="C345" t="s">
+        <v>592</v>
+      </c>
+      <c r="D345" t="s">
         <v>386</v>
-      </c>
-      <c r="C345" t="s">
-        <v>369</v>
-      </c>
-      <c r="D345" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
+        <v>387</v>
+      </c>
+      <c r="C346" t="s">
+        <v>592</v>
+      </c>
+      <c r="D346" t="s">
         <v>388</v>
-      </c>
-      <c r="C346" t="s">
-        <v>369</v>
-      </c>
-      <c r="D346" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
+        <v>389</v>
+      </c>
+      <c r="C347" t="s">
+        <v>592</v>
+      </c>
+      <c r="D347" t="s">
         <v>390</v>
-      </c>
-      <c r="C347" t="s">
-        <v>369</v>
-      </c>
-      <c r="D347" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
+        <v>391</v>
+      </c>
+      <c r="C348" t="s">
+        <v>592</v>
+      </c>
+      <c r="D348" t="s">
         <v>392</v>
-      </c>
-      <c r="C348" t="s">
-        <v>369</v>
-      </c>
-      <c r="D348" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
+        <v>393</v>
+      </c>
+      <c r="C349" t="s">
+        <v>592</v>
+      </c>
+      <c r="D349" t="s">
         <v>394</v>
-      </c>
-      <c r="C349" t="s">
-        <v>369</v>
-      </c>
-      <c r="D349" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C350" t="s">
-        <v>369</v>
+        <v>592</v>
       </c>
       <c r="D350" t="s">
         <v>165</v>
@@ -6716,560 +6719,563 @@
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
+        <v>396</v>
+      </c>
+      <c r="C351" t="s">
+        <v>592</v>
+      </c>
+      <c r="D351" t="s">
         <v>397</v>
-      </c>
-      <c r="C351" t="s">
-        <v>369</v>
-      </c>
-      <c r="D351" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
+        <v>398</v>
+      </c>
+      <c r="C352" t="s">
+        <v>581</v>
+      </c>
+      <c r="D352" t="s">
         <v>399</v>
       </c>
-      <c r="C352" t="s">
-        <v>582</v>
-      </c>
-      <c r="D352" t="s">
+    </row>
+    <row r="353" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A353" t="s">
+      <c r="C353" t="s">
+        <v>592</v>
+      </c>
+      <c r="D353" t="s">
         <v>401</v>
       </c>
-      <c r="C353" t="s">
-        <v>369</v>
-      </c>
-      <c r="D353" t="s">
+    </row>
+    <row r="354" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A354" t="s">
+      <c r="C354" t="s">
+        <v>592</v>
+      </c>
+      <c r="D354" t="s">
         <v>403</v>
       </c>
-      <c r="C354" t="s">
-        <v>369</v>
-      </c>
-      <c r="D354" t="s">
+    </row>
+    <row r="355" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A355" t="s">
+      <c r="C355" t="s">
+        <v>592</v>
+      </c>
+      <c r="D355" t="s">
         <v>405</v>
       </c>
-      <c r="C355" t="s">
-        <v>369</v>
-      </c>
-      <c r="D355" t="s">
+    </row>
+    <row r="356" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A356" t="s">
+      <c r="C356" t="s">
+        <v>592</v>
+      </c>
+      <c r="D356" t="s">
         <v>407</v>
       </c>
-      <c r="C356" t="s">
-        <v>369</v>
-      </c>
-      <c r="D356" t="s">
+    </row>
+    <row r="357" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A357" t="s">
+      <c r="C357" t="s">
+        <v>592</v>
+      </c>
+      <c r="D357" t="s">
         <v>409</v>
       </c>
-      <c r="C357" t="s">
-        <v>369</v>
-      </c>
-      <c r="D357" t="s">
+    </row>
+    <row r="358" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A358" t="s">
+      <c r="C358" t="s">
+        <v>586</v>
+      </c>
+      <c r="D358" t="s">
         <v>411</v>
       </c>
-      <c r="C358" t="s">
-        <v>587</v>
-      </c>
-      <c r="D358" t="s">
+    </row>
+    <row r="359" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A359" t="s">
+      <c r="C359" t="s">
+        <v>592</v>
+      </c>
+      <c r="D359" t="s">
         <v>413</v>
       </c>
-      <c r="C359" t="s">
-        <v>369</v>
-      </c>
-      <c r="D359" t="s">
+    </row>
+    <row r="360" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A360" t="s">
+      <c r="C360" t="s">
+        <v>592</v>
+      </c>
+      <c r="D360" t="s">
         <v>415</v>
       </c>
-      <c r="C360" t="s">
-        <v>369</v>
-      </c>
-      <c r="D360" t="s">
+    </row>
+    <row r="361" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A361" t="s">
+      <c r="C361" t="s">
+        <v>592</v>
+      </c>
+      <c r="D361" t="s">
         <v>417</v>
       </c>
-      <c r="C361" t="s">
-        <v>369</v>
-      </c>
-      <c r="D361" t="s">
+    </row>
+    <row r="362" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A362" t="s">
+      <c r="C362" t="s">
+        <v>592</v>
+      </c>
+      <c r="D362" t="s">
         <v>419</v>
       </c>
-      <c r="C362" t="s">
-        <v>369</v>
-      </c>
-      <c r="D362" t="s">
+    </row>
+    <row r="363" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A363" t="s">
+      <c r="C363" t="s">
+        <v>592</v>
+      </c>
+      <c r="D363" t="s">
         <v>421</v>
       </c>
-      <c r="C363" t="s">
-        <v>369</v>
-      </c>
-      <c r="D363" t="s">
+      <c r="P363" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="364" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A364" t="s">
+      <c r="C364" t="s">
+        <v>581</v>
+      </c>
+      <c r="D364" t="s">
         <v>423</v>
       </c>
-      <c r="C364" t="s">
-        <v>582</v>
-      </c>
-      <c r="D364" t="s">
+    </row>
+    <row r="365" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A365" t="s">
+      <c r="C365" t="s">
+        <v>592</v>
+      </c>
+      <c r="D365" t="s">
         <v>425</v>
       </c>
-      <c r="C365" t="s">
-        <v>369</v>
-      </c>
-      <c r="D365" t="s">
+    </row>
+    <row r="366" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A366" t="s">
+      <c r="C366" t="s">
+        <v>592</v>
+      </c>
+      <c r="D366" t="s">
         <v>427</v>
       </c>
-      <c r="C366" t="s">
-        <v>369</v>
-      </c>
-      <c r="D366" t="s">
+    </row>
+    <row r="367" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A367" t="s">
+      <c r="C367" t="s">
+        <v>592</v>
+      </c>
+      <c r="D367" t="s">
         <v>429</v>
       </c>
-      <c r="C367" t="s">
-        <v>369</v>
-      </c>
-      <c r="D367" t="s">
+    </row>
+    <row r="368" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A368" t="s">
+      <c r="C368" t="s">
+        <v>585</v>
+      </c>
+      <c r="D368" t="s">
         <v>431</v>
-      </c>
-      <c r="C368" t="s">
-        <v>586</v>
-      </c>
-      <c r="D368" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
+        <v>432</v>
+      </c>
+      <c r="C369" t="s">
+        <v>592</v>
+      </c>
+      <c r="D369" t="s">
         <v>433</v>
-      </c>
-      <c r="C369" t="s">
-        <v>369</v>
-      </c>
-      <c r="D369" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
+        <v>434</v>
+      </c>
+      <c r="C370" t="s">
+        <v>592</v>
+      </c>
+      <c r="D370" t="s">
         <v>435</v>
-      </c>
-      <c r="C370" t="s">
-        <v>369</v>
-      </c>
-      <c r="D370" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
+        <v>436</v>
+      </c>
+      <c r="C371" t="s">
+        <v>584</v>
+      </c>
+      <c r="D371" t="s">
         <v>437</v>
-      </c>
-      <c r="C371" t="s">
-        <v>585</v>
-      </c>
-      <c r="D371" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
+        <v>438</v>
+      </c>
+      <c r="C372" t="s">
+        <v>592</v>
+      </c>
+      <c r="D372" t="s">
         <v>439</v>
-      </c>
-      <c r="C372" t="s">
-        <v>369</v>
-      </c>
-      <c r="D372" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
+        <v>440</v>
+      </c>
+      <c r="C373" t="s">
+        <v>592</v>
+      </c>
+      <c r="D373" t="s">
         <v>441</v>
-      </c>
-      <c r="C373" t="s">
-        <v>369</v>
-      </c>
-      <c r="D373" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
+        <v>442</v>
+      </c>
+      <c r="C374" t="s">
+        <v>592</v>
+      </c>
+      <c r="D374" t="s">
         <v>443</v>
-      </c>
-      <c r="C374" t="s">
-        <v>369</v>
-      </c>
-      <c r="D374" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
+        <v>444</v>
+      </c>
+      <c r="C375" t="s">
+        <v>592</v>
+      </c>
+      <c r="D375" t="s">
         <v>445</v>
-      </c>
-      <c r="C375" t="s">
-        <v>369</v>
-      </c>
-      <c r="D375" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
+        <v>446</v>
+      </c>
+      <c r="C376" t="s">
+        <v>592</v>
+      </c>
+      <c r="D376" t="s">
         <v>447</v>
-      </c>
-      <c r="C376" t="s">
-        <v>369</v>
-      </c>
-      <c r="D376" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
+        <v>448</v>
+      </c>
+      <c r="C377" t="s">
+        <v>592</v>
+      </c>
+      <c r="D377" t="s">
         <v>449</v>
-      </c>
-      <c r="C377" t="s">
-        <v>369</v>
-      </c>
-      <c r="D377" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
+        <v>450</v>
+      </c>
+      <c r="C378" t="s">
+        <v>592</v>
+      </c>
+      <c r="D378" t="s">
         <v>451</v>
-      </c>
-      <c r="C378" t="s">
-        <v>369</v>
-      </c>
-      <c r="D378" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
+        <v>452</v>
+      </c>
+      <c r="C379" t="s">
+        <v>583</v>
+      </c>
+      <c r="D379" t="s">
         <v>453</v>
-      </c>
-      <c r="C379" t="s">
-        <v>584</v>
-      </c>
-      <c r="D379" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
+        <v>454</v>
+      </c>
+      <c r="C380" t="s">
+        <v>592</v>
+      </c>
+      <c r="D380" t="s">
         <v>455</v>
-      </c>
-      <c r="C380" t="s">
-        <v>369</v>
-      </c>
-      <c r="D380" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
+        <v>456</v>
+      </c>
+      <c r="C381" t="s">
+        <v>592</v>
+      </c>
+      <c r="D381" t="s">
         <v>457</v>
-      </c>
-      <c r="C381" t="s">
-        <v>369</v>
-      </c>
-      <c r="D381" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
+        <v>458</v>
+      </c>
+      <c r="C382" t="s">
+        <v>592</v>
+      </c>
+      <c r="D382" t="s">
         <v>459</v>
-      </c>
-      <c r="C382" t="s">
-        <v>369</v>
-      </c>
-      <c r="D382" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
+        <v>460</v>
+      </c>
+      <c r="C383" t="s">
+        <v>592</v>
+      </c>
+      <c r="D383" t="s">
         <v>461</v>
-      </c>
-      <c r="C383" t="s">
-        <v>369</v>
-      </c>
-      <c r="D383" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
+        <v>462</v>
+      </c>
+      <c r="C384" t="s">
+        <v>584</v>
+      </c>
+      <c r="D384" t="s">
         <v>463</v>
-      </c>
-      <c r="C384" t="s">
-        <v>585</v>
-      </c>
-      <c r="D384" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
+        <v>464</v>
+      </c>
+      <c r="C385" t="s">
+        <v>592</v>
+      </c>
+      <c r="D385" t="s">
         <v>465</v>
-      </c>
-      <c r="C385" t="s">
-        <v>369</v>
-      </c>
-      <c r="D385" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
+        <v>466</v>
+      </c>
+      <c r="C386" t="s">
+        <v>592</v>
+      </c>
+      <c r="D386" t="s">
         <v>467</v>
-      </c>
-      <c r="C386" t="s">
-        <v>369</v>
-      </c>
-      <c r="D386" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
+        <v>468</v>
+      </c>
+      <c r="C387" t="s">
+        <v>592</v>
+      </c>
+      <c r="D387" t="s">
         <v>469</v>
-      </c>
-      <c r="C387" t="s">
-        <v>369</v>
-      </c>
-      <c r="D387" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
+        <v>470</v>
+      </c>
+      <c r="C388" t="s">
+        <v>592</v>
+      </c>
+      <c r="D388" t="s">
         <v>471</v>
-      </c>
-      <c r="C388" t="s">
-        <v>369</v>
-      </c>
-      <c r="D388" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
+        <v>472</v>
+      </c>
+      <c r="C389" t="s">
+        <v>592</v>
+      </c>
+      <c r="D389" t="s">
         <v>473</v>
-      </c>
-      <c r="C389" t="s">
-        <v>369</v>
-      </c>
-      <c r="D389" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
+        <v>474</v>
+      </c>
+      <c r="C390" t="s">
+        <v>592</v>
+      </c>
+      <c r="D390" t="s">
         <v>475</v>
-      </c>
-      <c r="C390" t="s">
-        <v>369</v>
-      </c>
-      <c r="D390" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
+        <v>476</v>
+      </c>
+      <c r="C391" t="s">
+        <v>592</v>
+      </c>
+      <c r="D391" t="s">
         <v>477</v>
-      </c>
-      <c r="C391" t="s">
-        <v>369</v>
-      </c>
-      <c r="D391" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
+        <v>478</v>
+      </c>
+      <c r="C392" t="s">
+        <v>592</v>
+      </c>
+      <c r="D392" t="s">
         <v>479</v>
-      </c>
-      <c r="C392" t="s">
-        <v>369</v>
-      </c>
-      <c r="D392" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
+        <v>480</v>
+      </c>
+      <c r="C393" t="s">
+        <v>592</v>
+      </c>
+      <c r="D393" t="s">
         <v>481</v>
-      </c>
-      <c r="C393" t="s">
-        <v>369</v>
-      </c>
-      <c r="D393" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
+        <v>482</v>
+      </c>
+      <c r="C394" t="s">
+        <v>592</v>
+      </c>
+      <c r="D394" t="s">
         <v>483</v>
-      </c>
-      <c r="C394" t="s">
-        <v>369</v>
-      </c>
-      <c r="D394" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
+        <v>484</v>
+      </c>
+      <c r="C395" t="s">
+        <v>592</v>
+      </c>
+      <c r="D395" t="s">
         <v>485</v>
-      </c>
-      <c r="C395" t="s">
-        <v>369</v>
-      </c>
-      <c r="D395" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
+        <v>486</v>
+      </c>
+      <c r="C396" t="s">
+        <v>592</v>
+      </c>
+      <c r="D396" t="s">
         <v>487</v>
-      </c>
-      <c r="C396" t="s">
-        <v>369</v>
-      </c>
-      <c r="D396" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
+        <v>488</v>
+      </c>
+      <c r="C397" t="s">
+        <v>592</v>
+      </c>
+      <c r="D397" t="s">
         <v>489</v>
-      </c>
-      <c r="C397" t="s">
-        <v>369</v>
-      </c>
-      <c r="D397" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
+        <v>490</v>
+      </c>
+      <c r="C398" t="s">
+        <v>592</v>
+      </c>
+      <c r="D398" t="s">
         <v>491</v>
-      </c>
-      <c r="C398" t="s">
-        <v>369</v>
-      </c>
-      <c r="D398" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
+        <v>492</v>
+      </c>
+      <c r="C399" t="s">
+        <v>592</v>
+      </c>
+      <c r="D399" t="s">
         <v>493</v>
-      </c>
-      <c r="C399" t="s">
-        <v>369</v>
-      </c>
-      <c r="D399" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
+        <v>494</v>
+      </c>
+      <c r="C400" t="s">
+        <v>592</v>
+      </c>
+      <c r="D400" t="s">
         <v>495</v>
-      </c>
-      <c r="C400" t="s">
-        <v>369</v>
-      </c>
-      <c r="D400" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C401" t="s">
-        <v>369</v>
+        <v>592</v>
       </c>
       <c r="D401" t="s">
         <v>257</v>
@@ -7277,172 +7283,172 @@
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
+        <v>497</v>
+      </c>
+      <c r="C402" t="s">
+        <v>592</v>
+      </c>
+      <c r="D402" t="s">
         <v>498</v>
-      </c>
-      <c r="C402" t="s">
-        <v>369</v>
-      </c>
-      <c r="D402" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
+        <v>499</v>
+      </c>
+      <c r="C403" t="s">
+        <v>582</v>
+      </c>
+      <c r="D403" t="s">
         <v>500</v>
-      </c>
-      <c r="C403" t="s">
-        <v>583</v>
-      </c>
-      <c r="D403" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
+        <v>501</v>
+      </c>
+      <c r="C404" t="s">
+        <v>592</v>
+      </c>
+      <c r="D404" t="s">
         <v>502</v>
-      </c>
-      <c r="C404" t="s">
-        <v>369</v>
-      </c>
-      <c r="D404" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
+        <v>503</v>
+      </c>
+      <c r="C405" t="s">
+        <v>592</v>
+      </c>
+      <c r="D405" t="s">
         <v>504</v>
-      </c>
-      <c r="C405" t="s">
-        <v>369</v>
-      </c>
-      <c r="D405" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
+        <v>505</v>
+      </c>
+      <c r="C406" t="s">
+        <v>592</v>
+      </c>
+      <c r="D406" t="s">
         <v>506</v>
-      </c>
-      <c r="C406" t="s">
-        <v>369</v>
-      </c>
-      <c r="D406" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
+        <v>507</v>
+      </c>
+      <c r="C407" t="s">
+        <v>592</v>
+      </c>
+      <c r="D407" t="s">
         <v>508</v>
-      </c>
-      <c r="C407" t="s">
-        <v>369</v>
-      </c>
-      <c r="D407" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
+        <v>509</v>
+      </c>
+      <c r="C408" t="s">
+        <v>582</v>
+      </c>
+      <c r="D408" t="s">
         <v>510</v>
-      </c>
-      <c r="C408" t="s">
-        <v>583</v>
-      </c>
-      <c r="D408" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
+        <v>511</v>
+      </c>
+      <c r="C409" t="s">
+        <v>592</v>
+      </c>
+      <c r="D409" t="s">
         <v>512</v>
-      </c>
-      <c r="C409" t="s">
-        <v>369</v>
-      </c>
-      <c r="D409" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
+        <v>513</v>
+      </c>
+      <c r="C410" t="s">
+        <v>592</v>
+      </c>
+      <c r="D410" t="s">
         <v>514</v>
-      </c>
-      <c r="C410" t="s">
-        <v>369</v>
-      </c>
-      <c r="D410" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
+        <v>515</v>
+      </c>
+      <c r="C411" t="s">
+        <v>583</v>
+      </c>
+      <c r="D411" t="s">
         <v>516</v>
-      </c>
-      <c r="C411" t="s">
-        <v>584</v>
-      </c>
-      <c r="D411" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
+        <v>517</v>
+      </c>
+      <c r="C412" t="s">
+        <v>592</v>
+      </c>
+      <c r="D412" t="s">
         <v>518</v>
-      </c>
-      <c r="C412" t="s">
-        <v>369</v>
-      </c>
-      <c r="D412" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
+        <v>519</v>
+      </c>
+      <c r="C413" t="s">
+        <v>586</v>
+      </c>
+      <c r="D413" t="s">
         <v>520</v>
-      </c>
-      <c r="C413" t="s">
-        <v>587</v>
-      </c>
-      <c r="D413" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
+        <v>521</v>
+      </c>
+      <c r="C414" t="s">
+        <v>592</v>
+      </c>
+      <c r="D414" t="s">
         <v>522</v>
-      </c>
-      <c r="C414" t="s">
-        <v>369</v>
-      </c>
-      <c r="D414" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
+        <v>523</v>
+      </c>
+      <c r="C415" t="s">
+        <v>592</v>
+      </c>
+      <c r="D415" t="s">
         <v>524</v>
-      </c>
-      <c r="C415" t="s">
-        <v>369</v>
-      </c>
-      <c r="D415" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
+        <v>525</v>
+      </c>
+      <c r="C416" t="s">
+        <v>592</v>
+      </c>
+      <c r="D416" t="s">
         <v>526</v>
-      </c>
-      <c r="C416" t="s">
-        <v>369</v>
-      </c>
-      <c r="D416" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C417" t="s">
         <v>283</v>
@@ -7453,7 +7459,7 @@
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C418" t="s">
         <v>283</v>
@@ -7464,7 +7470,7 @@
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C419" t="s">
         <v>283</v>
@@ -7475,408 +7481,408 @@
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
+        <v>530</v>
+      </c>
+      <c r="B420" t="s">
+        <v>5</v>
+      </c>
+      <c r="C420" t="s">
+        <v>587</v>
+      </c>
+      <c r="D420" t="s">
         <v>531</v>
-      </c>
-      <c r="B420" t="s">
-        <v>5</v>
-      </c>
-      <c r="C420" t="s">
-        <v>588</v>
-      </c>
-      <c r="D420" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B421" t="s">
         <v>5</v>
       </c>
       <c r="C421" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D421" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B422" t="s">
         <v>5</v>
       </c>
       <c r="C422" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D422" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B423" t="s">
         <v>5</v>
       </c>
       <c r="C423" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D423" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B424" t="s">
         <v>5</v>
       </c>
       <c r="C424" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D424" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
+        <v>536</v>
+      </c>
+      <c r="B425" t="s">
+        <v>5</v>
+      </c>
+      <c r="C425" t="s">
+        <v>587</v>
+      </c>
+      <c r="D425" t="s">
         <v>537</v>
-      </c>
-      <c r="B425" t="s">
-        <v>5</v>
-      </c>
-      <c r="C425" t="s">
-        <v>588</v>
-      </c>
-      <c r="D425" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
+        <v>538</v>
+      </c>
+      <c r="B426" t="s">
+        <v>5</v>
+      </c>
+      <c r="C426" t="s">
+        <v>587</v>
+      </c>
+      <c r="D426" t="s">
         <v>539</v>
-      </c>
-      <c r="B426" t="s">
-        <v>5</v>
-      </c>
-      <c r="C426" t="s">
-        <v>588</v>
-      </c>
-      <c r="D426" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
+        <v>540</v>
+      </c>
+      <c r="B427" t="s">
+        <v>5</v>
+      </c>
+      <c r="C427" t="s">
+        <v>587</v>
+      </c>
+      <c r="D427" t="s">
         <v>541</v>
-      </c>
-      <c r="B427" t="s">
-        <v>5</v>
-      </c>
-      <c r="C427" t="s">
-        <v>588</v>
-      </c>
-      <c r="D427" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
+        <v>542</v>
+      </c>
+      <c r="B428" t="s">
+        <v>5</v>
+      </c>
+      <c r="C428" t="s">
+        <v>587</v>
+      </c>
+      <c r="D428" t="s">
         <v>543</v>
-      </c>
-      <c r="B428" t="s">
-        <v>5</v>
-      </c>
-      <c r="C428" t="s">
-        <v>588</v>
-      </c>
-      <c r="D428" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
+        <v>544</v>
+      </c>
+      <c r="B429" t="s">
+        <v>5</v>
+      </c>
+      <c r="C429" t="s">
+        <v>587</v>
+      </c>
+      <c r="D429" t="s">
         <v>545</v>
-      </c>
-      <c r="B429" t="s">
-        <v>5</v>
-      </c>
-      <c r="C429" t="s">
-        <v>588</v>
-      </c>
-      <c r="D429" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B430" t="s">
         <v>5</v>
       </c>
       <c r="C430" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D430" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B431" t="s">
         <v>5</v>
       </c>
       <c r="C431" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D431" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B432" t="s">
         <v>5</v>
       </c>
       <c r="C432" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D432" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B433" t="s">
         <v>5</v>
       </c>
       <c r="C433" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D433" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B434" t="s">
         <v>5</v>
       </c>
       <c r="C434" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D434" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
+        <v>551</v>
+      </c>
+      <c r="B435" t="s">
+        <v>5</v>
+      </c>
+      <c r="C435" t="s">
+        <v>587</v>
+      </c>
+      <c r="D435" t="s">
         <v>552</v>
-      </c>
-      <c r="B435" t="s">
-        <v>5</v>
-      </c>
-      <c r="C435" t="s">
-        <v>588</v>
-      </c>
-      <c r="D435" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
+        <v>553</v>
+      </c>
+      <c r="B436" t="s">
+        <v>5</v>
+      </c>
+      <c r="C436" t="s">
+        <v>587</v>
+      </c>
+      <c r="D436" t="s">
         <v>554</v>
-      </c>
-      <c r="B436" t="s">
-        <v>5</v>
-      </c>
-      <c r="C436" t="s">
-        <v>588</v>
-      </c>
-      <c r="D436" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B437" t="s">
         <v>5</v>
       </c>
       <c r="C437" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D437" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B438" t="s">
         <v>5</v>
       </c>
       <c r="C438" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D438" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B439" t="s">
         <v>5</v>
       </c>
       <c r="C439" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D439" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B440" t="s">
         <v>5</v>
       </c>
       <c r="C440" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D440" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B441" t="s">
         <v>5</v>
       </c>
       <c r="C441" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D441" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
+        <v>560</v>
+      </c>
+      <c r="B442" t="s">
         <v>561</v>
       </c>
-      <c r="B442" t="s">
+      <c r="C442" t="s">
         <v>562</v>
       </c>
-      <c r="C442" t="s">
+      <c r="D442" t="s">
         <v>563</v>
-      </c>
-      <c r="D442" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
+        <v>564</v>
+      </c>
+      <c r="B443" t="s">
         <v>565</v>
       </c>
-      <c r="B443" t="s">
+      <c r="C443" t="s">
         <v>566</v>
       </c>
-      <c r="C443" t="s">
+      <c r="D443" t="s">
         <v>567</v>
-      </c>
-      <c r="D443" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
+        <v>568</v>
+      </c>
+      <c r="B444" t="s">
+        <v>565</v>
+      </c>
+      <c r="C444" t="s">
+        <v>566</v>
+      </c>
+      <c r="D444" t="s">
         <v>569</v>
-      </c>
-      <c r="B444" t="s">
-        <v>566</v>
-      </c>
-      <c r="C444" t="s">
-        <v>567</v>
-      </c>
-      <c r="D444" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
+        <v>570</v>
+      </c>
+      <c r="B445" t="s">
         <v>571</v>
       </c>
-      <c r="B445" t="s">
+      <c r="C445" t="s">
         <v>572</v>
       </c>
-      <c r="C445" t="s">
+      <c r="D445" t="s">
         <v>573</v>
-      </c>
-      <c r="D445" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B446" t="s">
+        <v>565</v>
+      </c>
+      <c r="C446" t="s">
         <v>566</v>
       </c>
-      <c r="C446" t="s">
+      <c r="D446" t="s">
         <v>567</v>
-      </c>
-      <c r="D446" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
+        <v>575</v>
+      </c>
+      <c r="B447" t="s">
         <v>576</v>
       </c>
-      <c r="B447" t="s">
+      <c r="C447" t="s">
         <v>577</v>
       </c>
-      <c r="C447" t="s">
+      <c r="D447" t="s">
         <v>578</v>
-      </c>
-      <c r="D447" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
+        <v>579</v>
+      </c>
+      <c r="B448" t="s">
+        <v>5</v>
+      </c>
+      <c r="C448" t="s">
+        <v>591</v>
+      </c>
+      <c r="D448" t="s">
         <v>580</v>
-      </c>
-      <c r="B448" t="s">
-        <v>5</v>
-      </c>
-      <c r="C448" t="s">
-        <v>592</v>
-      </c>
-      <c r="D448" t="s">
-        <v>581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>